<commit_message>
Updated ReadMe file, also minor update to spreadsheet
</commit_message>
<xml_diff>
--- a/Spreadsheet_HAND_CatchID_ReachInfo.xlsx
+++ b/Spreadsheet_HAND_CatchID_ReachInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryan\Documents\GitHub\LiDAR_Processing\Floopldain_Inundation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5A711A74-F8EE-4530-953A-5C175BFBF342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{44D0B113-6FD0-4851-8B61-C5D341A5E655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-17025" yWindow="-13425" windowWidth="23505" windowHeight="11970"/>
   </bookViews>
@@ -914,7 +914,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C16" sqref="C16:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated spreadsheet so discharge is "flood_discharge_VIC_m3_sec" (instead of "Ten_year_flood_discharge..."), and updated ReadMe to reflect this language.
</commit_message>
<xml_diff>
--- a/Spreadsheet_HAND_CatchID_ReachInfo.xlsx
+++ b/Spreadsheet_HAND_CatchID_ReachInfo.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryan\Documents\GitHub\LiDAR_Processing\Floopldain_Inundation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{44D0B113-6FD0-4851-8B61-C5D341A5E655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE51803C-D039-4C5B-93CC-07DD6CBD8DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17025" yWindow="-13425" windowWidth="23505" windowHeight="11970"/>
+    <workbookView xWindow="-18525" yWindow="-14640" windowWidth="27075" windowHeight="13995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>Methow by central pivot in Big Valley</t>
   </si>
   <si>
-    <t>Ten_year_flood_VIC_m3_sec</t>
-  </si>
-  <si>
     <t>REM_Tif_Path</t>
   </si>
   <si>
@@ -68,12 +65,15 @@
   </si>
   <si>
     <t>P:/GIS/LiDAR/Methow_LiDAR/Methow_LiDAR/Methow_Texas_03_REM_WGS.tif</t>
+  </si>
+  <si>
+    <t>flood_discharge_VIC_m3_sec</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -910,11 +910,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:C17"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,22 +937,22 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -969,7 +969,7 @@
         <v>600</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2" s="1">
         <v>48.219275000000003</v>
@@ -998,7 +998,7 @@
         <v>600</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3">
         <v>48.206898000000002</v>
@@ -1027,7 +1027,7 @@
         <v>232</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" s="1">
         <v>48.498199999999997</v>
@@ -1056,7 +1056,7 @@
         <v>232</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5">
         <v>48.517349000000003</v>

</xml_diff>